<commit_message>
Menu Update/SD Card AutoInit Update
</commit_message>
<xml_diff>
--- a/Pangolin.xlsx
+++ b/Pangolin.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yagciilk\Documents\Arduino\Pangolin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D37E289B-36EB-49C1-B283-8A3299169082}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97BC19EB-F094-48A1-A124-F6BBBCAF9275}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Menu1" sheetId="1" r:id="rId1"/>
     <sheet name="Menu2" sheetId="2" r:id="rId2"/>
-    <sheet name="UI" sheetId="3" r:id="rId3"/>
+    <sheet name="Menu3" sheetId="4" r:id="rId3"/>
+    <sheet name="MenuF" sheetId="5" r:id="rId4"/>
+    <sheet name="UI" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="147">
   <si>
     <t xml:space="preserve">Enter </t>
   </si>
@@ -353,6 +355,129 @@
   </si>
   <si>
     <t>Index[4]</t>
+  </si>
+  <si>
+    <t>case(MENU4)</t>
+  </si>
+  <si>
+    <t>case(MENU5)</t>
+  </si>
+  <si>
+    <t>MENU4</t>
+  </si>
+  <si>
+    <t>MENU5</t>
+  </si>
+  <si>
+    <t>M5_SUB1</t>
+  </si>
+  <si>
+    <t>M5_SUB2</t>
+  </si>
+  <si>
+    <t>M5_SUB3</t>
+  </si>
+  <si>
+    <t>M5_SUB4</t>
+  </si>
+  <si>
+    <t>M5_SUB5</t>
+  </si>
+  <si>
+    <t>M5_SUB6</t>
+  </si>
+  <si>
+    <t>M5_SUB7</t>
+  </si>
+  <si>
+    <t>M4_SUB1</t>
+  </si>
+  <si>
+    <t>M4_SUB2</t>
+  </si>
+  <si>
+    <t>SUB1</t>
+  </si>
+  <si>
+    <t>SUB2</t>
+  </si>
+  <si>
+    <t>SUB33</t>
+  </si>
+  <si>
+    <t>SUB4</t>
+  </si>
+  <si>
+    <t>MENU6</t>
+  </si>
+  <si>
+    <t>MENU7</t>
+  </si>
+  <si>
+    <t>MENU8</t>
+  </si>
+  <si>
+    <t>SUB5</t>
+  </si>
+  <si>
+    <t>SUB6</t>
+  </si>
+  <si>
+    <t>SUB7</t>
+  </si>
+  <si>
+    <t>SUB8</t>
+  </si>
+  <si>
+    <t>SUB9</t>
+  </si>
+  <si>
+    <t>SUB10</t>
+  </si>
+  <si>
+    <t>SUB11</t>
+  </si>
+  <si>
+    <t>SUB12</t>
+  </si>
+  <si>
+    <t>SUB13</t>
+  </si>
+  <si>
+    <t>SUB14</t>
+  </si>
+  <si>
+    <t>SUB15</t>
+  </si>
+  <si>
+    <t>MENU9</t>
+  </si>
+  <si>
+    <t>MENU10</t>
+  </si>
+  <si>
+    <t>MENU11</t>
+  </si>
+  <si>
+    <t>MENU12</t>
+  </si>
+  <si>
+    <t>MENU13</t>
+  </si>
+  <si>
+    <t>MENU14</t>
+  </si>
+  <si>
+    <t>MENU15</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>MAIN</t>
+  </si>
+  <si>
+    <t>MENU</t>
   </si>
 </sst>
 </file>
@@ -568,6 +693,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
@@ -576,7 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -953,14 +1078,14 @@
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
         <v>3</v>
@@ -974,15 +1099,15 @@
       <c r="S4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="T4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="31"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -2128,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:AC44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2197,14 +2322,14 @@
       <c r="C4" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="27" t="s">
+      <c r="D4" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="27" t="s">
+      <c r="E4" s="29"/>
+      <c r="F4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="29"/>
       <c r="H4" s="21"/>
       <c r="I4" s="22" t="s">
         <v>3</v>
@@ -2227,15 +2352,15 @@
       <c r="S4" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="T4" s="29" t="s">
+      <c r="T4" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="U4" s="29"/>
-      <c r="V4" s="29"/>
-      <c r="W4" s="29"/>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="31"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B5">
@@ -3315,6 +3440,2231 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E648633-5BB0-4FFA-AB25-4F6B5B222844}">
+  <dimension ref="A2:AC44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O4" sqref="O4:P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="4.42578125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="6.140625" customWidth="1"/>
+    <col min="8" max="8" width="3.140625" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="11" max="11" width="10.5703125" customWidth="1"/>
+    <col min="12" max="12" width="6.28515625" customWidth="1"/>
+    <col min="15" max="15" width="18.28515625" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" style="5" customWidth="1"/>
+    <col min="17" max="17" width="4.42578125" customWidth="1"/>
+    <col min="18" max="18" width="18.5703125" customWidth="1"/>
+    <col min="19" max="19" width="14" style="2" customWidth="1"/>
+    <col min="20" max="20" width="16.28515625" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" style="2" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" style="2" customWidth="1"/>
+    <col min="23" max="23" width="8.140625" style="2" customWidth="1"/>
+    <col min="24" max="24" width="14.5703125" style="2" customWidth="1"/>
+    <col min="25" max="25" width="16.85546875" style="2" customWidth="1"/>
+    <col min="26" max="29" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="R2" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S2" s="8"/>
+      <c r="T2" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W2" s="8"/>
+      <c r="X2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y2" s="8"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>40</v>
+      </c>
+      <c r="O3" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="5">
+        <v>0</v>
+      </c>
+      <c r="R3" s="9"/>
+      <c r="S3" s="12"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="29"/>
+      <c r="F4" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="29"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N4" t="s">
+        <v>40</v>
+      </c>
+      <c r="O4" t="s">
+        <v>33</v>
+      </c>
+      <c r="P4" s="5">
+        <v>32</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="S4" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="T4" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="31"/>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>32</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="N5" t="s">
+        <v>40</v>
+      </c>
+      <c r="O5" t="s">
+        <v>34</v>
+      </c>
+      <c r="P5" s="5">
+        <v>64</v>
+      </c>
+      <c r="R5" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="S5" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T5" t="s">
+        <v>74</v>
+      </c>
+      <c r="U5" s="10"/>
+      <c r="V5" t="s">
+        <v>74</v>
+      </c>
+      <c r="X5" t="s">
+        <v>74</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" s="5">
+        <v>96</v>
+      </c>
+      <c r="R6" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="S6" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T6" t="s">
+        <v>75</v>
+      </c>
+      <c r="U6" s="10"/>
+      <c r="V6" t="s">
+        <v>75</v>
+      </c>
+      <c r="X6" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y6" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>32</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>64</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1">
+        <v>96</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>88</v>
+      </c>
+      <c r="N7" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" t="s">
+        <v>108</v>
+      </c>
+      <c r="P7" s="5">
+        <v>128</v>
+      </c>
+      <c r="R7" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T7" t="s">
+        <v>76</v>
+      </c>
+      <c r="U7" s="10"/>
+      <c r="V7" t="s">
+        <v>76</v>
+      </c>
+      <c r="X7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="3"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="N8" t="s">
+        <v>40</v>
+      </c>
+      <c r="O8" t="s">
+        <v>109</v>
+      </c>
+      <c r="P8" s="5">
+        <v>160</v>
+      </c>
+      <c r="R8" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="S8" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T8" t="s">
+        <v>106</v>
+      </c>
+      <c r="V8" t="s">
+        <v>106</v>
+      </c>
+      <c r="X8" t="s">
+        <v>106</v>
+      </c>
+      <c r="Y8" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>36</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1">
+        <v>4</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1">
+        <v>60</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="1">
+        <v>32</v>
+      </c>
+      <c r="J9" t="s">
+        <v>10</v>
+      </c>
+      <c r="R9" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="S9" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="T9" t="s">
+        <v>107</v>
+      </c>
+      <c r="V9" t="s">
+        <v>107</v>
+      </c>
+      <c r="X9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y9" s="10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>40</v>
+      </c>
+      <c r="C10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1">
+        <v>36</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="1">
+        <v>4</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="1">
+        <v>32</v>
+      </c>
+      <c r="J10" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" t="s">
+        <v>40</v>
+      </c>
+      <c r="O10" t="s">
+        <v>66</v>
+      </c>
+      <c r="P10" s="5">
+        <v>160</v>
+      </c>
+      <c r="R10" s="9"/>
+      <c r="S10" s="12"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>40</v>
+      </c>
+      <c r="O11" t="s">
+        <v>67</v>
+      </c>
+      <c r="P11" s="5">
+        <v>32</v>
+      </c>
+      <c r="R11" s="9"/>
+      <c r="S11" s="12"/>
+      <c r="U11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="W11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="T12" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="U12" s="13"/>
+      <c r="V12" s="10"/>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N13" t="s">
+        <v>40</v>
+      </c>
+      <c r="O13" t="s">
+        <v>37</v>
+      </c>
+      <c r="P13" s="5">
+        <v>36</v>
+      </c>
+      <c r="T13" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="U13" s="15"/>
+      <c r="V13" s="16"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="N14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" t="s">
+        <v>36</v>
+      </c>
+      <c r="P14" s="5">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16">
+        <v>64</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="1">
+        <v>96</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G16" s="1">
+        <v>32</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="1">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16" t="s">
+        <v>40</v>
+      </c>
+      <c r="O16" t="s">
+        <v>39</v>
+      </c>
+      <c r="P16" s="5">
+        <v>68</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S16" s="8"/>
+      <c r="T16" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W16" s="8"/>
+      <c r="X16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y16" s="8"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D17" s="3"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="N17" t="s">
+        <v>40</v>
+      </c>
+      <c r="O17" t="s">
+        <v>38</v>
+      </c>
+      <c r="P17" s="5">
+        <v>92</v>
+      </c>
+      <c r="R17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="S17" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="T17" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="U17" s="10"/>
+      <c r="V17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="W17" s="12"/>
+      <c r="X17" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y17" s="12"/>
+    </row>
+    <row r="18" spans="1:25" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18">
+        <v>68</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="1">
+        <v>4</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1">
+        <v>92</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="1">
+        <v>64</v>
+      </c>
+      <c r="J18">
+        <v>250</v>
+      </c>
+      <c r="K18" t="s">
+        <v>6</v>
+      </c>
+      <c r="R18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S18" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="T18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="U18" s="10"/>
+      <c r="V18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="W18" s="12"/>
+      <c r="X18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="Y18" s="12"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B19">
+        <v>72</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="1">
+        <v>4</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="1">
+        <v>64</v>
+      </c>
+      <c r="J19">
+        <v>500</v>
+      </c>
+      <c r="K19" t="s">
+        <v>6</v>
+      </c>
+      <c r="N19" t="s">
+        <v>40</v>
+      </c>
+      <c r="O19" t="s">
+        <v>65</v>
+      </c>
+      <c r="P19" s="5">
+        <v>100</v>
+      </c>
+      <c r="R19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="S19" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="T19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="U19" s="10"/>
+      <c r="V19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="W19" s="12"/>
+      <c r="X19" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y19" s="12"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <v>76</v>
+      </c>
+      <c r="C20" t="s">
+        <v>20</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1">
+        <v>4</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="1">
+        <v>4</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1">
+        <v>64</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+      <c r="N20" t="s">
+        <v>40</v>
+      </c>
+      <c r="O20" t="s">
+        <v>64</v>
+      </c>
+      <c r="P20" s="5">
+        <v>104</v>
+      </c>
+      <c r="R20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="S20" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="T20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="U20" s="10"/>
+      <c r="V20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="W20" s="12"/>
+      <c r="X20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="Y20" s="12"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B21">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1">
+        <v>4</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="1">
+        <v>4</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="1">
+        <v>64</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" t="s">
+        <v>8</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="S21" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="T21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="U21" s="10"/>
+      <c r="V21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="W21" s="12"/>
+      <c r="X21" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y21" s="12"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>84</v>
+      </c>
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="1">
+        <v>4</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="1">
+        <v>4</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I22" s="1">
+        <v>64</v>
+      </c>
+      <c r="J22">
+        <v>5</v>
+      </c>
+      <c r="K22" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="S22" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="T22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="U22" s="10"/>
+      <c r="V22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="W22" s="12"/>
+      <c r="X22" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="Y22" s="12"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>88</v>
+      </c>
+      <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="1">
+        <v>4</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="1">
+        <v>4</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I23" s="1">
+        <v>64</v>
+      </c>
+      <c r="J23">
+        <v>10</v>
+      </c>
+      <c r="K23" t="s">
+        <v>7</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="S23" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="T23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="U23" s="10"/>
+      <c r="V23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="W23" s="12"/>
+      <c r="X23" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="Y23" s="12"/>
+    </row>
+    <row r="24" spans="1:25" ht="12" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>92</v>
+      </c>
+      <c r="C24" t="s">
+        <v>24</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="1">
+        <v>68</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="1">
+        <v>4</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="1">
+        <v>64</v>
+      </c>
+      <c r="J24">
+        <v>20</v>
+      </c>
+      <c r="K24" t="s">
+        <v>7</v>
+      </c>
+      <c r="R24" s="9"/>
+      <c r="S24" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="T24" s="11"/>
+      <c r="U24" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="V24" s="10"/>
+      <c r="W24" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="12" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R25" s="9"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="U25" s="13"/>
+      <c r="V25" s="10"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="12"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R26" s="14"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="U26" s="15"/>
+      <c r="V26" s="16"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="20"/>
+      <c r="Y26" s="17"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="N27" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28">
+        <v>96</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="1">
+        <v>32</v>
+      </c>
+      <c r="F28" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="1">
+        <v>64</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0</v>
+      </c>
+      <c r="J28" t="s">
+        <v>12</v>
+      </c>
+      <c r="N28" t="s">
+        <v>63</v>
+      </c>
+      <c r="O28">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="D29" s="3"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="1">
+        <v>4</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G30" s="1">
+        <v>104</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I30" s="1">
+        <v>68</v>
+      </c>
+      <c r="J30" t="s">
+        <v>10</v>
+      </c>
+      <c r="L30" t="s">
+        <v>8</v>
+      </c>
+      <c r="R30" s="9"/>
+      <c r="S30" s="12"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="10"/>
+      <c r="V30" s="11"/>
+      <c r="W30" s="12"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="12"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B31">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="1">
+        <v>100</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="1">
+        <v>4</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I31" s="1">
+        <v>68</v>
+      </c>
+      <c r="J31" t="s">
+        <v>11</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="S31" s="8"/>
+      <c r="T31" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="W31" s="8"/>
+      <c r="X31" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y31" s="8"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="R32" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="S32" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="T32" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="U32" s="10"/>
+      <c r="V32" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="W32" s="12"/>
+      <c r="X32" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y32" s="12"/>
+    </row>
+    <row r="33" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="R33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="S33" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="T33" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="U33" s="10"/>
+      <c r="V33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="W33" s="12"/>
+      <c r="X33" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="Y33" s="12"/>
+    </row>
+    <row r="34" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="3"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="R34" s="9"/>
+      <c r="S34" s="12"/>
+      <c r="T34" s="11"/>
+      <c r="U34" s="10"/>
+      <c r="V34" s="11"/>
+      <c r="W34" s="12"/>
+      <c r="X34" s="9"/>
+      <c r="Y34" s="12"/>
+    </row>
+    <row r="35" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="D35" s="3"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="K35" t="s">
+        <v>48</v>
+      </c>
+      <c r="L35">
+        <v>36</v>
+      </c>
+      <c r="N35" t="s">
+        <v>110</v>
+      </c>
+      <c r="O35">
+        <v>164</v>
+      </c>
+      <c r="R35" s="9"/>
+      <c r="S35" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="T35" s="11"/>
+      <c r="U35" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="V35" s="10"/>
+      <c r="W35" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="X35" s="19"/>
+      <c r="Y35" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="F36" s="4"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="K36" t="s">
+        <v>49</v>
+      </c>
+      <c r="L36">
+        <v>40</v>
+      </c>
+      <c r="N36" t="s">
+        <v>111</v>
+      </c>
+      <c r="O36">
+        <v>168</v>
+      </c>
+      <c r="R36" s="9"/>
+      <c r="S36" s="12"/>
+      <c r="T36" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="U36" s="13"/>
+      <c r="V36" s="10"/>
+      <c r="W36" s="12"/>
+      <c r="X36" s="19"/>
+      <c r="Y36" s="12"/>
+    </row>
+    <row r="37" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="K37" t="s">
+        <v>50</v>
+      </c>
+      <c r="L37">
+        <v>44</v>
+      </c>
+      <c r="N37" t="s">
+        <v>112</v>
+      </c>
+      <c r="O37">
+        <v>172</v>
+      </c>
+      <c r="R37" s="14"/>
+      <c r="S37" s="17"/>
+      <c r="T37" s="25" t="s">
+        <v>69</v>
+      </c>
+      <c r="U37" s="15"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="17"/>
+      <c r="X37" s="20"/>
+      <c r="Y37" s="17"/>
+    </row>
+    <row r="38" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="K38" t="s">
+        <v>51</v>
+      </c>
+      <c r="L38">
+        <v>48</v>
+      </c>
+      <c r="N38" t="s">
+        <v>113</v>
+      </c>
+      <c r="O38">
+        <v>176</v>
+      </c>
+      <c r="U38" s="9" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="K39" t="s">
+        <v>52</v>
+      </c>
+      <c r="L39">
+        <v>52</v>
+      </c>
+      <c r="N39" t="s">
+        <v>114</v>
+      </c>
+      <c r="O39">
+        <v>180</v>
+      </c>
+      <c r="U39" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="40" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="K40" t="s">
+        <v>53</v>
+      </c>
+      <c r="L40">
+        <v>56</v>
+      </c>
+      <c r="N40" t="s">
+        <v>115</v>
+      </c>
+      <c r="O40">
+        <v>184</v>
+      </c>
+      <c r="U40" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="K41" t="s">
+        <v>54</v>
+      </c>
+      <c r="L41">
+        <v>60</v>
+      </c>
+      <c r="N41" t="s">
+        <v>116</v>
+      </c>
+      <c r="O41">
+        <v>188</v>
+      </c>
+      <c r="U41" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="U42" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="N43" t="s">
+        <v>117</v>
+      </c>
+      <c r="O43">
+        <v>132</v>
+      </c>
+      <c r="U43" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="44" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="N44" t="s">
+        <v>118</v>
+      </c>
+      <c r="O44">
+        <v>136</v>
+      </c>
+      <c r="U44" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="T4:Z4"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Classified as Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{90F7F362-1500-415B-8742-4DD6E6C5F9F7}">
+  <dimension ref="B3:R21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V24" sqref="V24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="5"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C3" s="5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="C4" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="D5" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="M5" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="O5" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="P5" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q5" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="R5" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="5">
+        <v>2</v>
+      </c>
+      <c r="F6" s="5">
+        <v>3</v>
+      </c>
+      <c r="G6" s="5">
+        <v>4</v>
+      </c>
+      <c r="H6" s="5">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>6</v>
+      </c>
+      <c r="J6" s="5">
+        <v>7</v>
+      </c>
+      <c r="K6" s="5">
+        <v>8</v>
+      </c>
+      <c r="L6" s="5">
+        <v>9</v>
+      </c>
+      <c r="M6" s="5">
+        <v>10</v>
+      </c>
+      <c r="N6" s="5">
+        <v>11</v>
+      </c>
+      <c r="O6" s="5">
+        <v>12</v>
+      </c>
+      <c r="P6" s="5">
+        <v>13</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>14</v>
+      </c>
+      <c r="R6" s="5">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B7" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="5">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5">
+        <v>17</v>
+      </c>
+      <c r="E7" s="5">
+        <v>18</v>
+      </c>
+      <c r="F7" s="5">
+        <v>19</v>
+      </c>
+      <c r="G7" s="5">
+        <v>20</v>
+      </c>
+      <c r="H7" s="5">
+        <v>21</v>
+      </c>
+      <c r="I7" s="5">
+        <v>22</v>
+      </c>
+      <c r="J7" s="5">
+        <v>23</v>
+      </c>
+      <c r="K7" s="5">
+        <v>24</v>
+      </c>
+      <c r="L7" s="5">
+        <v>25</v>
+      </c>
+      <c r="M7" s="5">
+        <v>26</v>
+      </c>
+      <c r="N7" s="5">
+        <v>27</v>
+      </c>
+      <c r="O7" s="5">
+        <v>28</v>
+      </c>
+      <c r="P7" s="5">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>30</v>
+      </c>
+      <c r="R7" s="5">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B8" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="5">
+        <v>32</v>
+      </c>
+      <c r="D8" s="5">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5">
+        <v>34</v>
+      </c>
+      <c r="F8" s="5">
+        <v>35</v>
+      </c>
+      <c r="G8" s="5">
+        <v>36</v>
+      </c>
+      <c r="H8" s="5">
+        <v>37</v>
+      </c>
+      <c r="I8" s="5">
+        <v>38</v>
+      </c>
+      <c r="J8" s="5">
+        <v>39</v>
+      </c>
+      <c r="K8" s="5">
+        <v>40</v>
+      </c>
+      <c r="L8" s="5">
+        <v>41</v>
+      </c>
+      <c r="M8" s="5">
+        <v>42</v>
+      </c>
+      <c r="N8" s="5">
+        <v>43</v>
+      </c>
+      <c r="O8" s="5">
+        <v>44</v>
+      </c>
+      <c r="P8" s="5">
+        <v>45</v>
+      </c>
+      <c r="Q8" s="5">
+        <v>46</v>
+      </c>
+      <c r="R8" s="5">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="5">
+        <v>48</v>
+      </c>
+      <c r="D9" s="5">
+        <v>49</v>
+      </c>
+      <c r="E9" s="5">
+        <v>50</v>
+      </c>
+      <c r="F9" s="5">
+        <v>51</v>
+      </c>
+      <c r="G9" s="5">
+        <v>52</v>
+      </c>
+      <c r="H9" s="5">
+        <v>53</v>
+      </c>
+      <c r="I9" s="5">
+        <v>54</v>
+      </c>
+      <c r="J9" s="5">
+        <v>55</v>
+      </c>
+      <c r="K9" s="5">
+        <v>56</v>
+      </c>
+      <c r="L9" s="5">
+        <v>57</v>
+      </c>
+      <c r="M9" s="5">
+        <v>58</v>
+      </c>
+      <c r="N9" s="5">
+        <v>59</v>
+      </c>
+      <c r="O9" s="5">
+        <v>60</v>
+      </c>
+      <c r="P9" s="5">
+        <v>61</v>
+      </c>
+      <c r="Q9" s="5">
+        <v>62</v>
+      </c>
+      <c r="R9" s="5">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="5">
+        <v>64</v>
+      </c>
+      <c r="D10" s="5">
+        <v>65</v>
+      </c>
+      <c r="E10" s="5">
+        <v>66</v>
+      </c>
+      <c r="F10" s="5">
+        <v>67</v>
+      </c>
+      <c r="G10" s="5">
+        <v>68</v>
+      </c>
+      <c r="H10" s="5">
+        <v>69</v>
+      </c>
+      <c r="I10" s="5">
+        <v>70</v>
+      </c>
+      <c r="J10" s="5">
+        <v>71</v>
+      </c>
+      <c r="K10" s="5">
+        <v>72</v>
+      </c>
+      <c r="L10" s="5">
+        <v>73</v>
+      </c>
+      <c r="M10" s="5">
+        <v>74</v>
+      </c>
+      <c r="N10" s="5">
+        <v>75</v>
+      </c>
+      <c r="O10" s="5">
+        <v>76</v>
+      </c>
+      <c r="P10" s="5">
+        <v>77</v>
+      </c>
+      <c r="Q10" s="5">
+        <v>78</v>
+      </c>
+      <c r="R10" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B11" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C11" s="5">
+        <v>80</v>
+      </c>
+      <c r="D11" s="5">
+        <v>81</v>
+      </c>
+      <c r="E11" s="5">
+        <v>82</v>
+      </c>
+      <c r="F11" s="5">
+        <v>83</v>
+      </c>
+      <c r="G11" s="5">
+        <v>84</v>
+      </c>
+      <c r="H11" s="5">
+        <v>85</v>
+      </c>
+      <c r="I11" s="5">
+        <v>86</v>
+      </c>
+      <c r="J11" s="5">
+        <v>87</v>
+      </c>
+      <c r="K11" s="5">
+        <v>88</v>
+      </c>
+      <c r="L11" s="5">
+        <v>89</v>
+      </c>
+      <c r="M11" s="5">
+        <v>90</v>
+      </c>
+      <c r="N11" s="5">
+        <v>91</v>
+      </c>
+      <c r="O11" s="5">
+        <v>92</v>
+      </c>
+      <c r="P11" s="5">
+        <v>93</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>94</v>
+      </c>
+      <c r="R11" s="5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C12" s="5">
+        <v>96</v>
+      </c>
+      <c r="D12" s="5">
+        <v>97</v>
+      </c>
+      <c r="E12" s="5">
+        <v>98</v>
+      </c>
+      <c r="F12" s="5">
+        <v>99</v>
+      </c>
+      <c r="G12" s="5">
+        <v>100</v>
+      </c>
+      <c r="H12" s="5">
+        <v>101</v>
+      </c>
+      <c r="I12" s="5">
+        <v>102</v>
+      </c>
+      <c r="J12" s="5">
+        <v>103</v>
+      </c>
+      <c r="K12" s="5">
+        <v>104</v>
+      </c>
+      <c r="L12" s="5">
+        <v>105</v>
+      </c>
+      <c r="M12" s="5">
+        <v>106</v>
+      </c>
+      <c r="N12" s="5">
+        <v>107</v>
+      </c>
+      <c r="O12" s="5">
+        <v>108</v>
+      </c>
+      <c r="P12" s="5">
+        <v>109</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>110</v>
+      </c>
+      <c r="R12" s="5">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B13" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C13" s="5">
+        <v>112</v>
+      </c>
+      <c r="D13" s="5">
+        <v>113</v>
+      </c>
+      <c r="E13" s="5">
+        <v>114</v>
+      </c>
+      <c r="F13" s="5">
+        <v>115</v>
+      </c>
+      <c r="G13" s="5">
+        <v>116</v>
+      </c>
+      <c r="H13" s="5">
+        <v>117</v>
+      </c>
+      <c r="I13" s="5">
+        <v>118</v>
+      </c>
+      <c r="J13" s="5">
+        <v>119</v>
+      </c>
+      <c r="K13" s="5">
+        <v>120</v>
+      </c>
+      <c r="L13" s="5">
+        <v>121</v>
+      </c>
+      <c r="M13" s="5">
+        <v>122</v>
+      </c>
+      <c r="N13" s="5">
+        <v>123</v>
+      </c>
+      <c r="O13" s="5">
+        <v>124</v>
+      </c>
+      <c r="P13" s="5">
+        <v>125</v>
+      </c>
+      <c r="Q13" s="5">
+        <v>126</v>
+      </c>
+      <c r="R13" s="5">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B14" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C14" s="5">
+        <v>128</v>
+      </c>
+      <c r="D14" s="5">
+        <v>129</v>
+      </c>
+      <c r="E14" s="5">
+        <v>130</v>
+      </c>
+      <c r="F14" s="5">
+        <v>131</v>
+      </c>
+      <c r="G14" s="5">
+        <v>132</v>
+      </c>
+      <c r="H14" s="5">
+        <v>133</v>
+      </c>
+      <c r="I14" s="5">
+        <v>134</v>
+      </c>
+      <c r="J14" s="5">
+        <v>135</v>
+      </c>
+      <c r="K14" s="5">
+        <v>136</v>
+      </c>
+      <c r="L14" s="5">
+        <v>137</v>
+      </c>
+      <c r="M14" s="5">
+        <v>138</v>
+      </c>
+      <c r="N14" s="5">
+        <v>139</v>
+      </c>
+      <c r="O14" s="5">
+        <v>140</v>
+      </c>
+      <c r="P14" s="5">
+        <v>141</v>
+      </c>
+      <c r="Q14" s="5">
+        <v>142</v>
+      </c>
+      <c r="R14" s="5">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B15" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C15" s="5">
+        <v>144</v>
+      </c>
+      <c r="D15" s="5">
+        <v>145</v>
+      </c>
+      <c r="E15" s="5">
+        <v>146</v>
+      </c>
+      <c r="F15" s="5">
+        <v>147</v>
+      </c>
+      <c r="G15" s="5">
+        <v>148</v>
+      </c>
+      <c r="H15" s="5">
+        <v>149</v>
+      </c>
+      <c r="I15" s="5">
+        <v>150</v>
+      </c>
+      <c r="J15" s="5">
+        <v>151</v>
+      </c>
+      <c r="K15" s="5">
+        <v>152</v>
+      </c>
+      <c r="L15" s="5">
+        <v>153</v>
+      </c>
+      <c r="M15" s="5">
+        <v>154</v>
+      </c>
+      <c r="N15" s="5">
+        <v>155</v>
+      </c>
+      <c r="O15" s="5">
+        <v>156</v>
+      </c>
+      <c r="P15" s="5">
+        <v>157</v>
+      </c>
+      <c r="Q15" s="5">
+        <v>158</v>
+      </c>
+      <c r="R15" s="5">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B16" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C16" s="5">
+        <v>160</v>
+      </c>
+      <c r="D16" s="5">
+        <v>161</v>
+      </c>
+      <c r="E16" s="5">
+        <v>162</v>
+      </c>
+      <c r="F16" s="5">
+        <v>163</v>
+      </c>
+      <c r="G16" s="5">
+        <v>164</v>
+      </c>
+      <c r="H16" s="5">
+        <v>165</v>
+      </c>
+      <c r="I16" s="5">
+        <v>166</v>
+      </c>
+      <c r="J16" s="5">
+        <v>167</v>
+      </c>
+      <c r="K16" s="5">
+        <v>168</v>
+      </c>
+      <c r="L16" s="5">
+        <v>169</v>
+      </c>
+      <c r="M16" s="5">
+        <v>170</v>
+      </c>
+      <c r="N16" s="5">
+        <v>171</v>
+      </c>
+      <c r="O16" s="5">
+        <v>172</v>
+      </c>
+      <c r="P16" s="5">
+        <v>173</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>174</v>
+      </c>
+      <c r="R16" s="5">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B17" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C17" s="5">
+        <v>176</v>
+      </c>
+      <c r="D17" s="5">
+        <v>177</v>
+      </c>
+      <c r="E17" s="5">
+        <v>178</v>
+      </c>
+      <c r="F17" s="5">
+        <v>179</v>
+      </c>
+      <c r="G17" s="5">
+        <v>180</v>
+      </c>
+      <c r="H17" s="5">
+        <v>181</v>
+      </c>
+      <c r="I17" s="5">
+        <v>182</v>
+      </c>
+      <c r="J17" s="5">
+        <v>183</v>
+      </c>
+      <c r="K17" s="5">
+        <v>184</v>
+      </c>
+      <c r="L17" s="5">
+        <v>185</v>
+      </c>
+      <c r="M17" s="5">
+        <v>186</v>
+      </c>
+      <c r="N17" s="5">
+        <v>187</v>
+      </c>
+      <c r="O17" s="5">
+        <v>188</v>
+      </c>
+      <c r="P17" s="5">
+        <v>189</v>
+      </c>
+      <c r="Q17" s="5">
+        <v>190</v>
+      </c>
+      <c r="R17" s="5">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B18" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="C18" s="5">
+        <v>192</v>
+      </c>
+      <c r="D18" s="5">
+        <v>193</v>
+      </c>
+      <c r="E18" s="5">
+        <v>194</v>
+      </c>
+      <c r="F18" s="5">
+        <v>195</v>
+      </c>
+      <c r="G18" s="5">
+        <v>196</v>
+      </c>
+      <c r="H18" s="5">
+        <v>197</v>
+      </c>
+      <c r="I18" s="5">
+        <v>198</v>
+      </c>
+      <c r="J18" s="5">
+        <v>199</v>
+      </c>
+      <c r="K18" s="5">
+        <v>200</v>
+      </c>
+      <c r="L18" s="5">
+        <v>201</v>
+      </c>
+      <c r="M18" s="5">
+        <v>202</v>
+      </c>
+      <c r="N18" s="5">
+        <v>203</v>
+      </c>
+      <c r="O18" s="5">
+        <v>204</v>
+      </c>
+      <c r="P18" s="5">
+        <v>205</v>
+      </c>
+      <c r="Q18" s="5">
+        <v>206</v>
+      </c>
+      <c r="R18" s="5">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C19" s="5">
+        <v>208</v>
+      </c>
+      <c r="D19" s="5">
+        <v>209</v>
+      </c>
+      <c r="E19" s="5">
+        <v>210</v>
+      </c>
+      <c r="F19" s="5">
+        <v>211</v>
+      </c>
+      <c r="G19" s="5">
+        <v>212</v>
+      </c>
+      <c r="H19" s="5">
+        <v>213</v>
+      </c>
+      <c r="I19" s="5">
+        <v>214</v>
+      </c>
+      <c r="J19" s="5">
+        <v>215</v>
+      </c>
+      <c r="K19" s="5">
+        <v>216</v>
+      </c>
+      <c r="L19" s="5">
+        <v>217</v>
+      </c>
+      <c r="M19" s="5">
+        <v>218</v>
+      </c>
+      <c r="N19" s="5">
+        <v>219</v>
+      </c>
+      <c r="O19" s="5">
+        <v>220</v>
+      </c>
+      <c r="P19" s="5">
+        <v>221</v>
+      </c>
+      <c r="Q19" s="5">
+        <v>222</v>
+      </c>
+      <c r="R19" s="5">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B20" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C20" s="5">
+        <v>224</v>
+      </c>
+      <c r="D20" s="5">
+        <v>225</v>
+      </c>
+      <c r="E20" s="5">
+        <v>226</v>
+      </c>
+      <c r="F20" s="5">
+        <v>227</v>
+      </c>
+      <c r="G20" s="5">
+        <v>228</v>
+      </c>
+      <c r="H20" s="5">
+        <v>229</v>
+      </c>
+      <c r="I20" s="5">
+        <v>230</v>
+      </c>
+      <c r="J20" s="5">
+        <v>231</v>
+      </c>
+      <c r="K20" s="5">
+        <v>232</v>
+      </c>
+      <c r="L20" s="5">
+        <v>233</v>
+      </c>
+      <c r="M20" s="5">
+        <v>234</v>
+      </c>
+      <c r="N20" s="5">
+        <v>235</v>
+      </c>
+      <c r="O20" s="5">
+        <v>236</v>
+      </c>
+      <c r="P20" s="5">
+        <v>237</v>
+      </c>
+      <c r="Q20" s="5">
+        <v>238</v>
+      </c>
+      <c r="R20" s="5">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C21" s="5">
+        <v>240</v>
+      </c>
+      <c r="D21" s="5">
+        <v>241</v>
+      </c>
+      <c r="E21" s="5">
+        <v>242</v>
+      </c>
+      <c r="F21" s="5">
+        <v>243</v>
+      </c>
+      <c r="G21" s="5">
+        <v>244</v>
+      </c>
+      <c r="H21" s="5">
+        <v>245</v>
+      </c>
+      <c r="I21" s="5">
+        <v>246</v>
+      </c>
+      <c r="J21" s="5">
+        <v>247</v>
+      </c>
+      <c r="K21" s="5">
+        <v>248</v>
+      </c>
+      <c r="L21" s="5">
+        <v>249</v>
+      </c>
+      <c r="M21" s="5">
+        <v>250</v>
+      </c>
+      <c r="N21" s="5">
+        <v>251</v>
+      </c>
+      <c r="O21" s="5">
+        <v>252</v>
+      </c>
+      <c r="P21" s="5">
+        <v>253</v>
+      </c>
+      <c r="Q21" s="5">
+        <v>254</v>
+      </c>
+      <c r="R21" s="5">
+        <v>255</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddFooter>&amp;L&amp;1#&amp;"Calibri"&amp;8&amp;K000000Classified as Internal</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2B68A86-94AC-4BD0-BF91-0EBCDE3F4854}">
   <dimension ref="A5:X23"/>
   <sheetViews>
@@ -3454,7 +5804,7 @@
       <c r="U10" t="s">
         <v>93</v>
       </c>
-      <c r="V10" s="31" t="s">
+      <c r="V10" s="27" t="s">
         <v>94</v>
       </c>
       <c r="W10" t="s">
@@ -3572,7 +5922,7 @@
       <c r="U12" t="s">
         <v>101</v>
       </c>
-      <c r="V12" s="31" t="s">
+      <c r="V12" s="27" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>